<commit_message>
Upgrade the SQL to one file with sheets
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -5,15 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snirb\PycharmProjects\Collind\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snirb\Dropbox\לימודים\סמי שמעון\שנה ב\סמסטר א\יסודות\פרויקט\Collind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D8C92F-9305-4B5C-AD18-70523F063479}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6ECA035-0EBA-43AD-8807-F95C9274355F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3940" yWindow="3800" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="17020" windowHeight="10120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Users" sheetId="4" r:id="rId1"/>
+    <sheet name="Cards" sheetId="1" r:id="rId2"/>
+    <sheet name="Games" sheetId="2" r:id="rId3"/>
+    <sheet name="Cube" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,12 +27,151 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>כוכב</t>
+  </si>
+  <si>
+    <t>עיגול</t>
+  </si>
+  <si>
+    <t>ריבוע</t>
+  </si>
+  <si>
+    <t>לב</t>
+  </si>
+  <si>
+    <t>ירח</t>
+  </si>
+  <si>
+    <t>משולש</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>CARD1</t>
+  </si>
+  <si>
+    <t>CARD2</t>
+  </si>
+  <si>
+    <t>CARD3</t>
+  </si>
+  <si>
+    <t>CARD4</t>
+  </si>
+  <si>
+    <t>CARD5</t>
+  </si>
+  <si>
+    <t>CARD6</t>
+  </si>
+  <si>
+    <t>CARD7</t>
+  </si>
+  <si>
+    <t>CARD8</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">correct </t>
+  </si>
+  <si>
+    <t>not correct</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Pic</t>
+  </si>
+  <si>
+    <t>Cube3</t>
+  </si>
+  <si>
+    <t>Cube4</t>
+  </si>
+  <si>
+    <t>Cube5</t>
+  </si>
+  <si>
+    <t>Cube6</t>
+  </si>
+  <si>
+    <t>Cube1.png</t>
+  </si>
+  <si>
+    <t>Cube2.png</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>team7</t>
+  </si>
+  <si>
+    <t>team7@gmail.com</t>
+  </si>
+  <si>
+    <t>UserId</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -43,7 +185,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -51,14 +193,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -336,136 +497,566 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE217E5-CDC7-4C6A-AF83-035779547E7E}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.58203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.4140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.9140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.9140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2">
+        <v>543149811</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{4C099850-EA83-4090-BC41-E1BF26F81E83}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>2</v>
-      </c>
-      <c r="B1">
-        <v>2</v>
-      </c>
-      <c r="C1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1">
-        <v>2</v>
-      </c>
-      <c r="E1">
-        <v>2</v>
-      </c>
-      <c r="F1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1">
+        <v>2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>4</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE22BC3-8BE4-4079-88ED-E3C05A6AAA47}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.58203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.4140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="D2">
+      <c r="B4">
         <v>4</v>
       </c>
-      <c r="E2">
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="F2">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="F6">
-        <v>6</v>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{907DEF6E-08E9-4485-95DE-94E07FE578ED}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.4140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>